<commit_message>
added test file and functions for reading in excel. Consistency check not working
</commit_message>
<xml_diff>
--- a/data/test_ahp.xlsx
+++ b/data/test_ahp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Ecology" sheetId="1" state="visible" r:id="rId2"/>
@@ -132,11 +132,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -200,11 +200,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -239,7 +239,8 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.1</v>
+        <f aca="false">1/9</f>
+        <v>0.111111111111111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>